<commit_message>
updating print id workbook
</commit_message>
<xml_diff>
--- a/Files/Print IDs.xlsx
+++ b/Files/Print IDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesmbp/Documents/GitHub/prodigi/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13513AE8-B577-244D-BD50-3CC697137769}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2446D9-2FA0-5C42-94AD-2F5B19B04C33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,7 +95,7 @@
     <t>Print Name</t>
   </si>
   <si>
-    <t>https://drive.google.com/open?id=1Tik7O5yXSrohqb0jOe80EC4tXYmzJKR1</t>
+    <t>https://drive.google.com/open?id=1Tik7O5yXSrohqb0jOe80EC4tXYmzJKRi</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -428,12 +428,12 @@
       <c r="B2" s="1">
         <v>123456789</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="2" t="str">
         <f>LEFT(C2,25)&amp;"uc?export=download&amp;"&amp;RIGHT(C2,LEN(C2)-30)</f>
-        <v>https://drive.google.com/uc?export=download&amp;id=1Tik7O5yXSrohqb0jOe80EC4tXYmzJKR1</v>
+        <v>https://drive.google.com/uc?export=download&amp;id=1Tik7O5yXSrohqb0jOe80EC4tXYmzJKRi</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -575,6 +575,9 @@
       <c r="D35" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{6D8B83AD-8C8D-F145-A6D0-3373DFA6D83B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>